<commit_message>
fiz merge do master e do code_smell_detection.
</commit_message>
<xml_diff>
--- a/src/main/Created_Excels/src_metrics.xlsx
+++ b/src/main/Created_Excels/src_metrics.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="73">
   <si>
     <t>MethodID</t>
   </si>
@@ -50,27 +50,33 @@
     <t>MQTTConnectionSender</t>
   </si>
   <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>is_god_class</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>islongmethod</t>
+  </si>
+  <si>
     <t>getMQTTSender</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>is_god_class</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>islongmethod</t>
-  </si>
-  <si>
     <t>getClient</t>
   </si>
   <si>
@@ -89,15 +95,18 @@
     <t>MQTTSender</t>
   </si>
   <si>
+    <t>addToList</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
     <t>removeFromList</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -110,36 +119,39 @@
     <t>MQTTConnection</t>
   </si>
   <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>receiveFromBroker</t>
   </si>
   <si>
-    <t>26</t>
-  </si>
-  <si>
     <t>MQTTImporter</t>
   </si>
   <si>
+    <t>getLimitesISCTE</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>218</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>getTable</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>218</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>24</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
     <t>start</t>
   </si>
   <si>
@@ -188,12 +200,12 @@
     <t>Task</t>
   </si>
   <si>
+    <t>212</t>
+  </si>
+  <si>
     <t>isDuplicate</t>
   </si>
   <si>
-    <t>212</t>
-  </si>
-  <si>
     <t>validateZone</t>
   </si>
   <si>
@@ -212,7 +224,13 @@
     <t>isValidDate</t>
   </si>
   <si>
-    <t>13</t>
+    <t>MongoToMongoTest</t>
+  </si>
+  <si>
+    <t>shouldAnswerWithTrue</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -303,15 +321,79 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -326,24 +408,56 @@
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
       </c>
       <c r="J4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -358,30 +472,62 @@
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
         <v>17</v>
       </c>
       <c r="J6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -390,39 +536,71 @@
         <v>15</v>
       </c>
       <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="I8" t="s">
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="J8" t="s">
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -433,127 +611,223 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
       <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
       <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="G11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="I11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>9.0</v>
+        <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="G13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>10.0</v>
+        <v>14.0</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="J17" t="s">
         <v>18</v>
@@ -561,28 +835,28 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
       <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" t="s">
-        <v>53</v>
       </c>
       <c r="I18" t="s">
         <v>17</v>
@@ -593,31 +867,31 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>12.0</v>
+        <v>18.0</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G19" t="s">
         <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="I19" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="J19" t="s">
         <v>18</v>
@@ -625,28 +899,28 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>16.0</v>
+        <v>19.0</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G20" t="s">
         <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I20" t="s">
         <v>17</v>
@@ -657,28 +931,28 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>13.0</v>
+        <v>20.0</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
         <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I21" t="s">
         <v>17</v>
@@ -689,28 +963,28 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
         <v>48</v>
-      </c>
-      <c r="D22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" t="s">
-        <v>29</v>
       </c>
       <c r="I22" t="s">
         <v>17</v>
@@ -721,31 +995,31 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>14.0</v>
+        <v>22.0</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
         <v>15</v>
       </c>
       <c r="H23" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="I23" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="J23" t="s">
         <v>18</v>
@@ -753,28 +1027,28 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>18.0</v>
+        <v>23.0</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G24" t="s">
         <v>15</v>
       </c>
       <c r="H24" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I24" t="s">
         <v>17</v>
@@ -785,31 +1059,31 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>22.0</v>
+        <v>24.0</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G25" t="s">
         <v>15</v>
       </c>
       <c r="H25" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="I25" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="J25" t="s">
         <v>18</v>
@@ -817,28 +1091,28 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>19.0</v>
+        <v>25.0</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E26" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G26" t="s">
         <v>15</v>
       </c>
       <c r="H26" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="I26" t="s">
         <v>17</v>
@@ -849,31 +1123,31 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>23.0</v>
+        <v>26.0</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="s">
         <v>60</v>
       </c>
-      <c r="D27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" t="s">
-        <v>20</v>
-      </c>
       <c r="I27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J27" t="s">
         <v>18</v>
@@ -881,31 +1155,31 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>20.0</v>
+        <v>27.0</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
         <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I28" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="J28" t="s">
         <v>18</v>
@@ -913,31 +1187,31 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>24.0</v>
+        <v>28.0</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G29" t="s">
         <v>15</v>
       </c>
       <c r="H29" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I29" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J29" t="s">
         <v>18</v>
@@ -945,31 +1219,31 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>21.0</v>
+        <v>29.0</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G30" t="s">
         <v>15</v>
       </c>
       <c r="H30" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I30" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J30" t="s">
         <v>18</v>
@@ -977,129 +1251,193 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>25.0</v>
+        <v>30.0</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" t="s">
         <v>62</v>
       </c>
-      <c r="D31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" t="s">
-        <v>59</v>
-      </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s">
         <v>15</v>
       </c>
       <c r="H31" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="I31" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="J31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>26.0</v>
+        <v>32.0</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D33" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F33" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G33" t="s">
         <v>15</v>
       </c>
       <c r="H33" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I33" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J34" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>27.0</v>
+        <v>34.0</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G35" t="s">
         <v>15</v>
       </c>
       <c r="H35" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I35" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="J35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="B37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" t="s">
-        <v>59</v>
-      </c>
-      <c r="F37" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" t="s">
-        <v>66</v>
-      </c>
-      <c r="I37" t="s">
-        <v>17</v>
-      </c>
-      <c r="J37" t="s">
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
From metrics to excel done.
</commit_message>
<xml_diff>
--- a/src/main/Created_Excels/src_metrics.xlsx
+++ b/src/main/Created_Excels/src_metrics.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="74">
   <si>
     <t>MethodID</t>
   </si>
@@ -47,6 +47,9 @@
     <t>is_Long_Method</t>
   </si>
   <si>
+    <t>org.pisid</t>
+  </si>
+  <si>
     <t>MQTTConnectionSender</t>
   </si>
   <si>
@@ -59,7 +62,7 @@
     <t>76</t>
   </si>
   <si>
-    <t>is_god_class</t>
+    <t>-</t>
   </si>
   <si>
     <t>4</t>
@@ -68,9 +71,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>islongmethod</t>
-  </si>
-  <si>
     <t>getMQTTSender</t>
   </si>
   <si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>run</t>
+  </si>
+  <si>
+    <t>org.pisid.mqtt_to_mysql</t>
   </si>
   <si>
     <t>MQTTConnection</t>
@@ -338,10 +341,10 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
@@ -351,6 +354,9 @@
       </c>
       <c r="J2" t="s">
         <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -361,28 +367,31 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
       <c r="J3" t="s">
         <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -393,28 +402,31 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
       <c r="J4" t="s">
         <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -425,28 +437,31 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
       <c r="J5" t="s">
         <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6">
@@ -457,28 +472,31 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
       <c r="J6" t="s">
         <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -486,22 +504,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
         <v>16</v>
@@ -511,6 +529,9 @@
       </c>
       <c r="J7" t="s">
         <v>18</v>
+      </c>
+      <c r="K7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -518,31 +539,34 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
         <v>31</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>32</v>
       </c>
-      <c r="J8" t="s">
-        <v>18</v>
+      <c r="K8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -550,31 +574,34 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
         <v>22</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>32</v>
       </c>
-      <c r="J9" t="s">
-        <v>18</v>
+      <c r="K9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -585,28 +612,31 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
         <v>32</v>
       </c>
-      <c r="G10" t="s">
-        <v>15</v>
-      </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="J10" t="s">
         <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -617,28 +647,31 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
         <v>32</v>
       </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
       <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
         <v>32</v>
       </c>
-      <c r="G11" t="s">
-        <v>15</v>
-      </c>
       <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
         <v>28</v>
       </c>
-      <c r="I11" t="s">
-        <v>17</v>
-      </c>
       <c r="J11" t="s">
         <v>18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12">
@@ -646,7 +679,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
@@ -661,16 +694,19 @@
         <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="J12" t="s">
         <v>18</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13">
@@ -678,13 +714,13 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
         <v>41</v>
@@ -693,16 +729,19 @@
         <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H13" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="J13" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14">
@@ -710,13 +749,13 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
         <v>41</v>
@@ -725,7 +764,7 @@
         <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H14" t="s">
         <v>16</v>
@@ -735,6 +774,9 @@
       </c>
       <c r="J14" t="s">
         <v>18</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15">
@@ -742,13 +784,13 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
@@ -757,7 +799,7 @@
         <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H15" t="s">
         <v>16</v>
@@ -767,6 +809,9 @@
       </c>
       <c r="J15" t="s">
         <v>18</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16">
@@ -774,13 +819,13 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
         <v>41</v>
@@ -789,16 +834,19 @@
         <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H16" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="J16" t="s">
         <v>18</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17">
@@ -806,13 +854,13 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>40</v>
       </c>
       <c r="E17" t="s">
         <v>41</v>
@@ -821,16 +869,19 @@
         <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="I17" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" t="s">
         <v>32</v>
       </c>
-      <c r="J17" t="s">
-        <v>18</v>
+      <c r="K17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -838,13 +889,13 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
@@ -853,16 +904,19 @@
         <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H18" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="J18" t="s">
         <v>18</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19">
@@ -870,13 +924,13 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
         <v>41</v>
@@ -885,16 +939,19 @@
         <v>42</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="I19" t="s">
         <v>54</v>
       </c>
       <c r="J19" t="s">
-        <v>18</v>
+        <v>55</v>
+      </c>
+      <c r="K19" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20">
@@ -902,22 +959,22 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" t="s">
         <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" t="s">
-        <v>15</v>
       </c>
       <c r="H20" t="s">
         <v>16</v>
@@ -927,6 +984,9 @@
       </c>
       <c r="J20" t="s">
         <v>18</v>
+      </c>
+      <c r="K20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21">
@@ -934,31 +994,34 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" t="s">
         <v>55</v>
       </c>
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" t="s">
-        <v>15</v>
-      </c>
       <c r="H21" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="I21" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="J21" t="s">
         <v>18</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22">
@@ -966,31 +1029,34 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" t="s">
-        <v>15</v>
-      </c>
       <c r="H22" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I22" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="J22" t="s">
         <v>18</v>
+      </c>
+      <c r="K22" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23">
@@ -998,31 +1064,34 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" t="s">
         <v>55</v>
       </c>
-      <c r="C23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" t="s">
-        <v>15</v>
-      </c>
       <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
         <v>32</v>
       </c>
-      <c r="I23" t="s">
-        <v>17</v>
-      </c>
       <c r="J23" t="s">
         <v>18</v>
+      </c>
+      <c r="K23" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24">
@@ -1030,31 +1099,34 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" t="s">
         <v>55</v>
       </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" t="s">
-        <v>15</v>
-      </c>
       <c r="H24" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I24" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="J24" t="s">
         <v>18</v>
+      </c>
+      <c r="K24" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25">
@@ -1062,22 +1134,22 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" t="s">
         <v>55</v>
-      </c>
-      <c r="C25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" t="s">
-        <v>15</v>
       </c>
       <c r="H25" t="s">
         <v>16</v>
@@ -1087,6 +1159,9 @@
       </c>
       <c r="J25" t="s">
         <v>18</v>
+      </c>
+      <c r="K25" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26">
@@ -1094,31 +1169,34 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" t="s">
         <v>55</v>
       </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26" t="s">
-        <v>15</v>
-      </c>
       <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" t="s">
         <v>24</v>
       </c>
-      <c r="I26" t="s">
-        <v>17</v>
-      </c>
       <c r="J26" t="s">
         <v>18</v>
+      </c>
+      <c r="K26" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27">
@@ -1126,31 +1204,34 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" t="s">
         <v>55</v>
       </c>
-      <c r="C27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" t="s">
-        <v>15</v>
-      </c>
       <c r="H27" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="I27" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" t="s">
         <v>28</v>
       </c>
-      <c r="J27" t="s">
-        <v>18</v>
+      <c r="K27" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28">
@@ -1158,31 +1239,34 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
         <v>33</v>
       </c>
-      <c r="D28" t="s">
-        <v>40</v>
-      </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H28" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" t="s">
         <v>29</v>
       </c>
-      <c r="I28" t="s">
-        <v>40</v>
-      </c>
       <c r="J28" t="s">
-        <v>18</v>
+        <v>41</v>
+      </c>
+      <c r="K28" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29">
@@ -1190,31 +1274,34 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" t="s">
         <v>63</v>
       </c>
-      <c r="D29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" t="s">
-        <v>42</v>
-      </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H29" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="I29" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" t="s">
         <v>32</v>
       </c>
-      <c r="J29" t="s">
-        <v>18</v>
+      <c r="K29" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="30">
@@ -1222,31 +1309,34 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" t="s">
         <v>22</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>32</v>
       </c>
-      <c r="J30" t="s">
-        <v>18</v>
+      <c r="K30" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="31">
@@ -1254,31 +1344,34 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E31" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="F31" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H31" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="I31" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" t="s">
         <v>28</v>
       </c>
-      <c r="J31" t="s">
-        <v>18</v>
+      <c r="K31" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32">
@@ -1286,31 +1379,34 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E32" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H32" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I32" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="J32" t="s">
         <v>18</v>
+      </c>
+      <c r="K32" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="33">
@@ -1318,31 +1414,34 @@
         <v>32.0</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="E33" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="F33" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" t="s">
         <v>24</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>32</v>
       </c>
-      <c r="J33" t="s">
-        <v>18</v>
+      <c r="K33" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="34">
@@ -1350,31 +1449,34 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H34" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I34" t="s">
+        <v>41</v>
+      </c>
+      <c r="J34" t="s">
         <v>32</v>
       </c>
-      <c r="J34" t="s">
-        <v>18</v>
+      <c r="K34" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="35">
@@ -1382,31 +1484,34 @@
         <v>34.0</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="F35" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H35" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="I35" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="J35" t="s">
         <v>18</v>
+      </c>
+      <c r="K35" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="36">
@@ -1414,31 +1519,34 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
         <v>71</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="E36" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="F36" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" t="s">
         <v>28</v>
       </c>
-      <c r="I36" t="s">
-        <v>17</v>
-      </c>
       <c r="J36" t="s">
         <v>18</v>
+      </c>
+      <c r="K36" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>